<commit_message>
update spring 2023 sample times
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Spring2023.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Spring2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive - University of Idaho\Desktop\Research\La Jara Data\LISST GSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C211704B-6023-4758-8096-0C4CAC9975B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC52E5AF-9546-45EE-B83E-2E1A8B727EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{99C89BF0-5701-4EDE-976A-2DC8AC06B2E1}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{99C89BF0-5701-4EDE-976A-2DC8AC06B2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="ISCO 1 (down)" sheetId="1" r:id="rId1"/>
@@ -1329,6 +1329,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1348,15 +1357,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1675,46 +1675,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4F41F3-2406-4DBC-AD18-012969672032}">
   <dimension ref="A2:O152"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="D15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="I2" s="29" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="I2" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="16" t="s">
@@ -1750,7 +1750,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>141</v>
       </c>
       <c r="J4" s="3">
-        <v>45033</v>
+        <v>45033.6875</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
@@ -1794,7 +1794,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>124</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>144</v>
       </c>
       <c r="J5" s="3">
-        <v>45033</v>
+        <v>45033.854166666664</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -1839,7 +1839,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>131</v>
       </c>
@@ -1864,8 +1864,8 @@
       <c r="I6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="21">
-        <v>45034</v>
+      <c r="J6" s="3">
+        <v>45034.020833333336</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
@@ -1883,7 +1883,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>110</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>110</v>
       </c>
       <c r="J7" s="3">
-        <v>45034</v>
+        <v>45034.1875</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
@@ -1927,7 +1927,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>175</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>96</v>
       </c>
       <c r="J8" s="3">
-        <v>45034</v>
+        <v>45034.354166666664</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -1971,7 +1971,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>177</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>131</v>
       </c>
       <c r="J9" s="3">
-        <v>45034</v>
+        <v>45034.520833333336</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -2016,7 +2016,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>192</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>117</v>
       </c>
       <c r="J10" s="9">
-        <v>45034</v>
+        <v>45034.6875</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
@@ -2061,7 +2061,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>199</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>114</v>
       </c>
       <c r="J11" s="9">
-        <v>45034</v>
+        <v>45034.895833333336</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
@@ -2106,7 +2106,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>127</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>129</v>
       </c>
       <c r="J12" s="9">
-        <v>45035</v>
+        <v>45035.104166666664</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>144</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>120</v>
       </c>
       <c r="J13" s="3">
-        <v>45035</v>
+        <v>45035.3125</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
@@ -2199,7 +2199,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>120</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>109</v>
       </c>
       <c r="J14" s="3">
-        <v>45035</v>
+        <v>45035.520833333336</v>
       </c>
       <c r="K14" s="2">
         <v>0</v>
@@ -2244,7 +2244,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>135</v>
       </c>
       <c r="J15" s="9">
-        <v>45036</v>
+        <v>45036.666666666664</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
@@ -2289,7 +2289,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>194</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>127</v>
       </c>
       <c r="J16" s="3">
-        <v>45036</v>
+        <v>45036.770833333336</v>
       </c>
       <c r="K16" s="2">
         <v>0</v>
@@ -2334,7 +2334,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>117</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>121</v>
       </c>
       <c r="J17" s="9">
-        <v>45036</v>
+        <v>45036.979166666664</v>
       </c>
       <c r="K17" s="2">
         <v>0</v>
@@ -2379,7 +2379,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>141</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>138</v>
       </c>
       <c r="J18" s="9">
-        <v>45037</v>
+        <v>45037.1875</v>
       </c>
       <c r="K18" s="2">
         <v>0</v>
@@ -2424,7 +2424,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>134</v>
       </c>
       <c r="J19" s="9">
-        <v>45037</v>
+        <v>45037.395833333336</v>
       </c>
       <c r="K19" s="2">
         <v>0</v>
@@ -2469,7 +2469,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>114</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>141</v>
       </c>
       <c r="J20" s="9">
-        <v>45037</v>
+        <v>45037.604166666664</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
@@ -2514,7 +2514,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>134</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>119</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>96</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>196</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>201</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>109</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>138</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>121</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>179</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>184</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>186</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>144</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>94</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>110</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>96</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>131</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>136</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>143</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>91</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>117</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>182</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>92</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>120</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>129</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>109</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>135</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>108</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>121</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>127</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>138</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>94</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>134</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>141</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>144</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>110</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>131</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>91</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>112</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>114</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>117</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>119</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>92</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>108</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>109</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>108</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>120</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>121</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>124</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>127</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>129</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>114</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>220</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>221</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>222</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>114</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>227</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>229</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>135</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>109</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>141</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>117</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>232</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>234</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>236</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>129</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>138</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>134</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>238</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>240</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>242</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>121</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>129</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>245</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>247</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>249</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>120</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -5518,7 +5518,7 @@
       <c r="F101"/>
       <c r="G101"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -5527,7 +5527,7 @@
       <c r="F102"/>
       <c r="G102"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -5536,7 +5536,7 @@
       <c r="F103"/>
       <c r="G103"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -5545,7 +5545,7 @@
       <c r="F104"/>
       <c r="G104"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -5554,7 +5554,7 @@
       <c r="F105"/>
       <c r="G105"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -5563,7 +5563,7 @@
       <c r="F106"/>
       <c r="G106"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -5572,7 +5572,7 @@
       <c r="F107"/>
       <c r="G107"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -5581,7 +5581,7 @@
       <c r="F108"/>
       <c r="G108"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -5590,7 +5590,7 @@
       <c r="F109"/>
       <c r="G109"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -5599,7 +5599,7 @@
       <c r="F110"/>
       <c r="G110"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -5608,7 +5608,7 @@
       <c r="F111"/>
       <c r="G111"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -5617,46 +5617,46 @@
       <c r="F112"/>
       <c r="G112"/>
     </row>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="150" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="151" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="152" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A3:N100" xr:uid="{DC4F41F3-2406-4DBC-AD18-012969672032}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N100">
@@ -5675,35 +5675,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47770336-139B-4E1D-B90D-A41F00945441}">
   <dimension ref="A2:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="17.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5546875" customWidth="1"/>
-    <col min="15" max="15" width="19.5546875" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="6">
+        <v>45040</v>
+      </c>
+      <c r="L2" s="2">
+        <v>253</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="23">
+        <v>96.2</v>
+      </c>
+      <c r="O2" s="23">
+        <v>27.12</v>
+      </c>
+      <c r="P2" s="23">
+        <v>48.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
@@ -5719,10 +5741,10 @@
       <c r="G3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="30" t="s">
         <v>337</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -5741,7 +5763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -5763,29 +5785,29 @@
       <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="3">
-        <v>45033</v>
+      <c r="J4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="9">
+        <v>45033.6875</v>
       </c>
       <c r="L4" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <v>97.05</v>
+        <v>93.4</v>
       </c>
       <c r="O4" s="23">
-        <v>73.675000000000011</v>
+        <v>103.30500000000001</v>
       </c>
       <c r="P4" s="23">
-        <v>91.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>81.800000000000011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -5807,29 +5829,29 @@
       <c r="G5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" s="9">
-        <v>45033</v>
+      <c r="J5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="15">
+        <v>45033.854166666664</v>
       </c>
       <c r="L5" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M5" s="2">
         <v>0</v>
       </c>
       <c r="N5" s="23">
-        <v>93.4</v>
+        <v>94.4</v>
       </c>
       <c r="O5" s="23">
-        <v>103.30500000000001</v>
+        <v>65.48</v>
       </c>
       <c r="P5" s="23">
-        <v>81.800000000000011</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>51.72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -5851,29 +5873,29 @@
       <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="K6" s="15">
-        <v>45033</v>
+      <c r="J6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="3">
+        <v>45034.020833333336</v>
       </c>
       <c r="L6" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M6" s="2">
         <v>0</v>
       </c>
       <c r="N6" s="23">
-        <v>94.4</v>
+        <v>97.05</v>
       </c>
       <c r="O6" s="23">
-        <v>65.48</v>
+        <v>73.675000000000011</v>
       </c>
       <c r="P6" s="23">
-        <v>51.72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>91.46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -5895,32 +5917,32 @@
       <c r="G7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="3">
-        <v>45034</v>
-      </c>
-      <c r="L7" s="38">
-        <v>211</v>
+      <c r="J7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="9">
+        <v>45034.1875</v>
+      </c>
+      <c r="L7" s="2">
+        <v>193</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>64</v>
+      <c r="N7" s="23">
+        <v>96.9</v>
       </c>
       <c r="O7" s="23">
-        <v>0</v>
+        <v>48.895000000000003</v>
       </c>
       <c r="P7" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>58.709999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>14</v>
       </c>
@@ -5942,30 +5964,30 @@
       <c r="G8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="J8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" s="9">
-        <v>45034</v>
-      </c>
-      <c r="L8" s="2">
-        <v>193</v>
+      <c r="H8" s="37"/>
+      <c r="J8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="3">
+        <v>45034.354166666664</v>
+      </c>
+      <c r="L8" s="31">
+        <v>211</v>
       </c>
       <c r="M8" s="2">
         <v>0</v>
       </c>
-      <c r="N8" s="23">
-        <v>96.9</v>
+      <c r="N8" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="O8" s="23">
-        <v>48.895000000000003</v>
+        <v>0</v>
       </c>
       <c r="P8" s="23">
-        <v>58.709999999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>16</v>
       </c>
@@ -5987,12 +6009,12 @@
       <c r="G9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="34"/>
+      <c r="H9" s="37"/>
       <c r="J9" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K9" s="9">
-        <v>45034</v>
+        <v>45034.520833333336</v>
       </c>
       <c r="L9" s="2">
         <v>212</v>
@@ -6010,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
@@ -6032,12 +6054,12 @@
       <c r="G10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="34"/>
+      <c r="H10" s="37"/>
       <c r="J10" s="2" t="s">
         <v>69</v>
       </c>
       <c r="K10" s="9">
-        <v>45034</v>
+        <v>45034.6875</v>
       </c>
       <c r="L10" s="2">
         <v>213</v>
@@ -6055,7 +6077,7 @@
         <v>56.024999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
@@ -6077,12 +6099,12 @@
       <c r="G11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="37"/>
       <c r="J11" s="12" t="s">
         <v>142</v>
       </c>
       <c r="K11" s="13">
-        <v>45034</v>
+        <v>45034.895833333336</v>
       </c>
       <c r="L11" s="2">
         <v>214</v>
@@ -6100,7 +6122,7 @@
         <v>66.137500000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -6122,30 +6144,30 @@
       <c r="G12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="34"/>
-      <c r="J12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="K12" s="6">
-        <v>45035</v>
+      <c r="H12" s="37"/>
+      <c r="J12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="9">
+        <v>45035.104166666664</v>
       </c>
       <c r="L12" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="M12" s="2">
         <v>0</v>
       </c>
       <c r="N12" s="23">
-        <v>96.800000000000011</v>
+        <v>96.633333333333326</v>
       </c>
       <c r="O12" s="23">
-        <v>22.36</v>
+        <v>47.579999999999991</v>
       </c>
       <c r="P12" s="23">
-        <v>38.814999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>57.156666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>26</v>
       </c>
@@ -6167,30 +6189,30 @@
       <c r="G13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="J13" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K13" s="6">
-        <v>45035</v>
+      <c r="H13" s="37"/>
+      <c r="J13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="9">
+        <v>45035.3125</v>
       </c>
       <c r="L13" s="2">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
       </c>
-      <c r="N13" s="23" t="s">
-        <v>64</v>
+      <c r="N13" s="23">
+        <v>97.066666666666677</v>
       </c>
       <c r="O13" s="23">
-        <v>0</v>
+        <v>30.72</v>
       </c>
       <c r="P13" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>47.137500000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>27</v>
       </c>
@@ -6212,30 +6234,30 @@
       <c r="G14" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="J14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="9">
-        <v>45035</v>
+      <c r="H14" s="37"/>
+      <c r="J14" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" s="11">
+        <v>45035.520833333336</v>
       </c>
       <c r="L14" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
       </c>
-      <c r="N14" s="23">
-        <v>97.066666666666677</v>
+      <c r="N14" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="O14" s="23">
-        <v>30.72</v>
+        <v>0</v>
       </c>
       <c r="P14" s="23">
-        <v>47.137500000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>28</v>
       </c>
@@ -6257,30 +6279,30 @@
       <c r="G15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="34"/>
-      <c r="J15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" s="9">
-        <v>45035</v>
+      <c r="H15" s="37"/>
+      <c r="J15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" s="6">
+        <v>45035.729166666664</v>
       </c>
       <c r="L15" s="2">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="M15" s="2">
         <v>0</v>
       </c>
-      <c r="N15" s="23">
-        <v>96.633333333333326</v>
+      <c r="N15" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="O15" s="23">
-        <v>47.579999999999991</v>
+        <v>0</v>
       </c>
       <c r="P15" s="23">
-        <v>57.156666666666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>29</v>
       </c>
@@ -6302,30 +6324,30 @@
       <c r="G16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="34"/>
-      <c r="J16" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="K16" s="11">
-        <v>45035</v>
+      <c r="H16" s="37"/>
+      <c r="J16" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="6">
+        <v>45035.9375</v>
       </c>
       <c r="L16" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="M16" s="2">
         <v>0</v>
       </c>
-      <c r="N16" s="23" t="s">
-        <v>68</v>
+      <c r="N16" s="23">
+        <v>96.800000000000011</v>
       </c>
       <c r="O16" s="23">
-        <v>0</v>
+        <v>22.36</v>
       </c>
       <c r="P16" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>38.814999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>30</v>
       </c>
@@ -6347,30 +6369,30 @@
       <c r="G17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="34"/>
-      <c r="J17" s="7" t="s">
-        <v>9</v>
+      <c r="H17" s="37"/>
+      <c r="J17" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="K17" s="6">
-        <v>45036</v>
+        <v>45036.145833333336</v>
       </c>
       <c r="L17" s="2">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="M17" s="2">
         <v>0</v>
       </c>
       <c r="N17" s="23">
-        <v>97</v>
+        <v>96.8</v>
       </c>
       <c r="O17" s="23">
-        <v>24.91</v>
+        <v>30.83</v>
       </c>
       <c r="P17" s="23">
-        <v>58.21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>40</v>
       </c>
@@ -6392,30 +6414,30 @@
       <c r="G18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="J18" s="5" t="s">
-        <v>115</v>
+      <c r="H18" s="37"/>
+      <c r="J18" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="K18" s="6">
-        <v>45036</v>
+        <v>45036.354166666664</v>
       </c>
       <c r="L18" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M18" s="2">
         <v>0</v>
       </c>
-      <c r="N18" s="23">
-        <v>96.8</v>
+      <c r="N18" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="O18" s="23">
-        <v>30.83</v>
+        <v>0</v>
       </c>
       <c r="P18" s="23">
-        <v>52.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>41</v>
       </c>
@@ -6437,15 +6459,15 @@
       <c r="G19" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="34"/>
+      <c r="H19" s="37"/>
       <c r="J19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" s="6">
-        <v>45036</v>
+        <v>104</v>
+      </c>
+      <c r="K19" s="9">
+        <v>45036.770833333336</v>
       </c>
       <c r="L19" s="2">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -6460,7 +6482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>42</v>
       </c>
@@ -6482,30 +6504,30 @@
       <c r="G20" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="J20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K20" s="9">
-        <v>45036</v>
+      <c r="H20" s="37"/>
+      <c r="J20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="6">
+        <v>45036.979166666664</v>
       </c>
       <c r="L20" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M20" s="2">
         <v>0</v>
       </c>
-      <c r="N20" s="23" t="s">
-        <v>64</v>
+      <c r="N20" s="23">
+        <v>97</v>
       </c>
       <c r="O20" s="23">
-        <v>0</v>
+        <v>24.91</v>
       </c>
       <c r="P20" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>58.21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>43</v>
       </c>
@@ -6527,12 +6549,12 @@
       <c r="G21" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="34"/>
+      <c r="H21" s="37"/>
       <c r="J21" s="7" t="s">
         <v>81</v>
       </c>
       <c r="K21" s="6">
-        <v>45037</v>
+        <v>45037.395833333336</v>
       </c>
       <c r="L21" s="2">
         <v>238</v>
@@ -6550,7 +6572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>44</v>
       </c>
@@ -6572,12 +6594,12 @@
       <c r="G22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="34"/>
+      <c r="H22" s="37"/>
       <c r="J22" s="7" t="s">
         <v>95</v>
       </c>
       <c r="K22" s="6">
-        <v>45037</v>
+        <v>45037.604166666664</v>
       </c>
       <c r="L22" s="2">
         <v>239</v>
@@ -6595,7 +6617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>45</v>
       </c>
@@ -6617,12 +6639,12 @@
       <c r="G23" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="34"/>
+      <c r="H23" s="37"/>
       <c r="J23" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K23" s="13">
-        <v>45037</v>
+        <v>45037.8125</v>
       </c>
       <c r="L23" s="2">
         <v>240</v>
@@ -6640,7 +6662,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>47</v>
       </c>
@@ -6662,30 +6684,30 @@
       <c r="G24" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="34"/>
-      <c r="J24" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="K24" s="11">
-        <v>45038</v>
+      <c r="H24" s="37"/>
+      <c r="J24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K24" s="15">
+        <v>45038.020833333336</v>
       </c>
       <c r="L24" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M24" s="2">
         <v>0</v>
       </c>
-      <c r="N24" s="23">
-        <v>96.974999999999994</v>
+      <c r="N24" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="O24" s="23">
-        <v>51.682499999999997</v>
+        <v>0</v>
       </c>
       <c r="P24" s="23">
-        <v>80.920000000000016</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>48</v>
       </c>
@@ -6707,30 +6729,30 @@
       <c r="G25" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="34"/>
+      <c r="H25" s="37"/>
       <c r="J25" s="10" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="K25" s="11">
-        <v>45038</v>
+        <v>45038.229166666664</v>
       </c>
       <c r="L25" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M25" s="2">
         <v>0</v>
       </c>
-      <c r="N25" s="23" t="s">
-        <v>68</v>
+      <c r="N25" s="23">
+        <v>96.974999999999994</v>
       </c>
       <c r="O25" s="23">
-        <v>0</v>
+        <v>51.682499999999997</v>
       </c>
       <c r="P25" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80.920000000000016</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -6752,32 +6774,32 @@
       <c r="G26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="K26" s="15">
-        <v>45038</v>
+      <c r="J26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K26" s="11">
+        <v>45038.4375</v>
       </c>
       <c r="L26" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M26" s="2">
         <v>0</v>
       </c>
-      <c r="N26" s="23">
-        <v>96.333333333333329</v>
+      <c r="N26" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="O26" s="23">
-        <v>57.56</v>
+        <v>0</v>
       </c>
       <c r="P26" s="23">
-        <v>65.026666666666657</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>52</v>
       </c>
@@ -6799,30 +6821,30 @@
       <c r="G27" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="31"/>
-      <c r="J27" s="2" t="s">
-        <v>113</v>
+      <c r="H27" s="34"/>
+      <c r="J27" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="K27" s="15">
-        <v>45038</v>
+        <v>45038.645833333336</v>
       </c>
       <c r="L27" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M27" s="2">
         <v>0</v>
       </c>
-      <c r="N27" s="23" t="s">
-        <v>68</v>
+      <c r="N27" s="23">
+        <v>96.333333333333329</v>
       </c>
       <c r="O27" s="23">
-        <v>0</v>
+        <v>57.56</v>
       </c>
       <c r="P27" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+        <v>65.026666666666657</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>55</v>
       </c>
@@ -6844,30 +6866,30 @@
       <c r="G28" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H28" s="31"/>
-      <c r="J28" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" s="6">
-        <v>45039</v>
+      <c r="H28" s="34"/>
+      <c r="J28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="11">
+        <v>45038.854166666664</v>
       </c>
       <c r="L28" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M28" s="2">
         <v>0</v>
       </c>
-      <c r="N28" s="23" t="s">
-        <v>64</v>
+      <c r="N28" s="23">
+        <v>95.375000000000014</v>
       </c>
       <c r="O28" s="23">
-        <v>0</v>
+        <v>63.535000000000011</v>
       </c>
       <c r="P28" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+        <v>59.204999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>59</v>
       </c>
@@ -6889,15 +6911,15 @@
       <c r="G29" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H29" s="31"/>
-      <c r="J29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K29" s="11">
-        <v>45039</v>
+      <c r="H29" s="34"/>
+      <c r="J29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="15">
+        <v>45039.0625</v>
       </c>
       <c r="L29" s="2">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M29" s="2">
         <v>0</v>
@@ -6912,7 +6934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>61</v>
       </c>
@@ -6934,30 +6956,30 @@
       <c r="G30" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="31"/>
-      <c r="J30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K30" s="11">
-        <v>45039</v>
+      <c r="H30" s="34"/>
+      <c r="J30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K30" s="13">
+        <v>45039.479166666664</v>
       </c>
       <c r="L30" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="M30" s="2">
         <v>0</v>
       </c>
-      <c r="N30" s="23">
-        <v>95.375000000000014</v>
+      <c r="N30" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="O30" s="23">
-        <v>63.535000000000011</v>
+        <v>0</v>
       </c>
       <c r="P30" s="23">
-        <v>59.204999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -6981,13 +7003,13 @@
       </c>
       <c r="H31" s="20"/>
       <c r="J31" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="K31" s="13">
+        <v>69</v>
+      </c>
+      <c r="K31" s="11">
         <v>45039</v>
       </c>
       <c r="L31" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M31" s="2">
         <v>0</v>
@@ -7002,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -7025,20 +7047,20 @@
         <v>66</v>
       </c>
       <c r="H32" s="20"/>
-      <c r="J32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="15">
+      <c r="J32" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K32" s="6">
         <v>45039</v>
       </c>
       <c r="L32" s="2">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M32" s="2">
         <v>0</v>
       </c>
       <c r="N32" s="23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O32" s="23">
         <v>0</v>
@@ -7047,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -7069,29 +7091,29 @@
       <c r="G33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J33" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="K33" s="6">
+      <c r="J33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="9">
         <v>45040</v>
       </c>
       <c r="L33" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
       </c>
       <c r="N33" s="23">
-        <v>96.2</v>
+        <v>97.3</v>
       </c>
       <c r="O33" s="23">
-        <v>27.12</v>
+        <v>66.586666666666673</v>
       </c>
       <c r="P33" s="23">
-        <v>48.05</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+        <v>69.806666666666658</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>69</v>
       </c>
@@ -7138,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>71</v>
       </c>
@@ -7160,29 +7182,29 @@
       <c r="G35" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J35" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="K35" s="6">
+      <c r="J35" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="K35" s="15">
         <v>45040</v>
       </c>
       <c r="L35" s="2">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="M35" s="2">
         <v>0</v>
       </c>
       <c r="N35" s="23">
-        <v>97.05</v>
+        <v>96.533333333333346</v>
       </c>
       <c r="O35" s="23">
-        <v>14.59</v>
+        <v>46.75</v>
       </c>
       <c r="P35" s="23">
-        <v>25.344999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+        <v>59.133333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>75</v>
       </c>
@@ -7207,29 +7229,29 @@
       <c r="H36" t="s">
         <v>74</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K36" s="9">
-        <v>45040</v>
+      <c r="J36" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K36" s="6">
+        <v>45041</v>
       </c>
       <c r="L36" s="2">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="M36" s="2">
         <v>0</v>
       </c>
-      <c r="N36" s="23">
-        <v>97.3</v>
+      <c r="N36" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="O36" s="23">
-        <v>66.586666666666673</v>
+        <v>0</v>
       </c>
       <c r="P36" s="23">
-        <v>69.806666666666658</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>77</v>
       </c>
@@ -7251,29 +7273,29 @@
       <c r="G37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="K37" s="15">
+      <c r="J37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K37" s="6">
         <v>45040</v>
       </c>
       <c r="L37" s="2">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="M37" s="2">
         <v>0</v>
       </c>
       <c r="N37" s="23">
-        <v>96.533333333333346</v>
+        <v>97.05</v>
       </c>
       <c r="O37" s="23">
-        <v>46.75</v>
+        <v>14.59</v>
       </c>
       <c r="P37" s="23">
-        <v>59.133333333333333</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+        <v>25.344999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>80</v>
       </c>
@@ -7295,14 +7317,14 @@
       <c r="G38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J38" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K38" s="6">
+      <c r="J38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K38" s="9">
         <v>45041</v>
       </c>
       <c r="L38" s="2">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M38" s="2">
         <v>0</v>
@@ -7317,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>81</v>
       </c>
@@ -7339,29 +7361,8 @@
       <c r="G39" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K39" s="9">
-        <v>45041</v>
-      </c>
-      <c r="L39" s="2">
-        <v>270</v>
-      </c>
-      <c r="M39" s="2">
-        <v>0</v>
-      </c>
-      <c r="N39" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O39" s="23">
-        <v>0</v>
-      </c>
-      <c r="P39" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>83</v>
       </c>
@@ -7405,7 +7406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>85</v>
       </c>
@@ -7449,7 +7450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>87</v>
       </c>
@@ -7493,7 +7494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>88</v>
       </c>
@@ -7537,7 +7538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>89</v>
       </c>
@@ -7581,7 +7582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
@@ -7625,7 +7626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>77</v>
       </c>
@@ -7669,7 +7670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
@@ -7713,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>99</v>
       </c>
@@ -7757,7 +7758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>101</v>
       </c>
@@ -7801,7 +7802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>102</v>
       </c>
@@ -7845,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>104</v>
       </c>
@@ -7889,7 +7890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>106</v>
       </c>
@@ -7933,7 +7934,7 @@
         <v>47.98</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -7977,7 +7978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>115</v>
       </c>
@@ -8021,7 +8022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>123</v>
       </c>
@@ -8065,7 +8066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>106</v>
       </c>
@@ -8109,7 +8110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -8153,7 +8154,7 @@
         <v>79.88</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>81</v>
       </c>
@@ -8197,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>115</v>
       </c>
@@ -8241,7 +8242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>133</v>
       </c>
@@ -8285,7 +8286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>140</v>
       </c>
@@ -8329,7 +8330,7 @@
         <v>53.17</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>102</v>
       </c>
@@ -8373,7 +8374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>51</v>
       </c>
@@ -8417,7 +8418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>95</v>
       </c>
@@ -8461,7 +8462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>142</v>
       </c>
@@ -8505,7 +8506,7 @@
         <v>87.02</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>9</v>
       </c>
@@ -8549,7 +8550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>102</v>
       </c>
@@ -8593,7 +8594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>9</v>
       </c>
@@ -8637,7 +8638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>87</v>
       </c>
@@ -8681,7 +8682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>88</v>
       </c>
@@ -8725,7 +8726,7 @@
         <v>54.92</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>142</v>
       </c>
@@ -8769,7 +8770,7 @@
         <v>49.949999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>104</v>
       </c>
@@ -8813,7 +8814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>89</v>
       </c>
@@ -8857,7 +8858,7 @@
         <v>30.57</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>81</v>
       </c>
@@ -8901,7 +8902,7 @@
         <v>26.823333333333334</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>87</v>
       </c>
@@ -8945,7 +8946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>152</v>
       </c>
@@ -8989,7 +8990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>115</v>
       </c>
@@ -9033,7 +9034,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>102</v>
       </c>
@@ -9077,7 +9078,7 @@
         <v>133.34</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -9121,7 +9122,7 @@
         <v>79.66</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>113</v>
       </c>
@@ -9165,7 +9166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>95</v>
       </c>
@@ -9209,7 +9210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>95</v>
       </c>
@@ -9253,7 +9254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>104</v>
       </c>
@@ -9297,7 +9298,7 @@
         <v>50.42</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>133</v>
       </c>
@@ -9341,7 +9342,7 @@
         <v>44.193333333333328</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>101</v>
       </c>
@@ -9385,7 +9386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>77</v>
       </c>
@@ -9429,7 +9430,7 @@
         <v>113.11</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>10</v>
       </c>
@@ -9473,7 +9474,7 @@
         <v>93.39</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>8</v>
       </c>
@@ -9496,7 +9497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>155</v>
       </c>
@@ -9519,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -9542,7 +9543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>156</v>
       </c>
@@ -9565,7 +9566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>123</v>
       </c>
@@ -9588,7 +9589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>142</v>
       </c>
@@ -9611,7 +9612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>69</v>
       </c>
@@ -9634,7 +9635,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>71</v>
       </c>
@@ -9657,7 +9658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>75</v>
       </c>
@@ -9680,7 +9681,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>159</v>
       </c>
@@ -9703,7 +9704,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>99</v>
       </c>
@@ -9726,7 +9727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>101</v>
       </c>
@@ -9749,7 +9750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>77</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>80</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>161</v>
       </c>
@@ -9818,7 +9819,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>165</v>
       </c>
@@ -9841,7 +9842,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>113</v>
       </c>
@@ -9864,7 +9865,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>168</v>
       </c>
@@ -9887,7 +9888,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>170</v>
       </c>
@@ -9910,7 +9911,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>172</v>
       </c>
@@ -9933,7 +9934,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>133</v>
       </c>
@@ -9956,7 +9957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>81</v>
       </c>
@@ -9979,7 +9980,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>83</v>
       </c>
@@ -10002,7 +10003,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>115</v>
       </c>
@@ -10025,7 +10026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>62</v>
       </c>
@@ -10048,7 +10049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>104</v>
       </c>
@@ -10071,7 +10072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>99</v>
       </c>
@@ -10094,7 +10095,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>204</v>
       </c>
@@ -10117,7 +10118,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>206</v>
       </c>
@@ -10140,7 +10141,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>89</v>
       </c>
@@ -10163,7 +10164,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>209</v>
       </c>
@@ -10186,7 +10187,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>211</v>
       </c>
@@ -10209,7 +10210,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>213</v>
       </c>
@@ -10232,7 +10233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>99</v>
       </c>
@@ -10255,7 +10256,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>204</v>
       </c>
@@ -10278,7 +10279,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>206</v>
       </c>
@@ -10301,7 +10302,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>69</v>
       </c>
@@ -10324,7 +10325,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>71</v>
       </c>
@@ -10347,7 +10348,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>69</v>
       </c>
@@ -10370,7 +10371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>101</v>
       </c>
@@ -10393,7 +10394,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>252</v>
       </c>
@@ -10416,7 +10417,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>254</v>
       </c>
@@ -10439,7 +10440,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="s">
         <v>256</v>
       </c>
@@ -10462,7 +10463,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>123</v>
       </c>
@@ -10485,7 +10486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>8</v>
       </c>
@@ -10508,7 +10509,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>259</v>
       </c>
@@ -10531,7 +10532,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>261</v>
       </c>
@@ -10554,7 +10555,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>263</v>
       </c>
@@ -10577,7 +10578,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>133</v>
       </c>
@@ -10600,7 +10601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>156</v>
       </c>
@@ -10623,7 +10624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>265</v>
       </c>
@@ -10646,7 +10647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>142</v>
       </c>
@@ -10669,7 +10670,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>267</v>
       </c>
@@ -10692,7 +10693,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>269</v>
       </c>
@@ -10715,7 +10716,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
         <v>271</v>
       </c>
@@ -10738,7 +10739,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
         <v>95</v>
       </c>
@@ -10761,7 +10762,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
         <v>274</v>
       </c>
@@ -10784,7 +10785,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
         <v>276</v>
       </c>
@@ -10807,7 +10808,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
         <v>278</v>
       </c>
@@ -10830,7 +10831,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
         <v>123</v>
       </c>
@@ -10853,7 +10854,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
         <v>281</v>
       </c>
@@ -10876,7 +10877,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
         <v>283</v>
       </c>
@@ -10899,7 +10900,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
         <v>10</v>
       </c>
@@ -10922,7 +10923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
         <v>90</v>
       </c>
@@ -10945,7 +10946,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
         <v>286</v>
       </c>
@@ -10968,7 +10969,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
         <v>288</v>
       </c>
@@ -10991,7 +10992,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>113</v>
       </c>
@@ -11014,7 +11015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>77</v>
       </c>
@@ -11037,7 +11038,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
         <v>80</v>
       </c>
@@ -11085,20 +11086,20 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
@@ -11115,7 +11116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>292</v>
       </c>
@@ -11138,7 +11139,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>294</v>
       </c>
@@ -11161,7 +11162,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>296</v>
       </c>
@@ -11184,7 +11185,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>298</v>
       </c>
@@ -11207,7 +11208,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>299</v>
       </c>
@@ -11230,7 +11231,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>301</v>
       </c>
@@ -11253,7 +11254,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>304</v>
       </c>
@@ -11276,7 +11277,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>306</v>
       </c>
@@ -11299,7 +11300,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>308</v>
       </c>
@@ -11322,7 +11323,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>310</v>
       </c>
@@ -11345,7 +11346,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>312</v>
       </c>
@@ -11368,7 +11369,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>314</v>
       </c>
@@ -11391,7 +11392,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>316</v>
       </c>
@@ -11414,7 +11415,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>318</v>
       </c>
@@ -11437,7 +11438,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>320</v>
       </c>
@@ -11460,7 +11461,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>322</v>
       </c>
@@ -11483,7 +11484,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>324</v>
       </c>
@@ -11506,7 +11507,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>326</v>
       </c>
@@ -11529,7 +11530,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>328</v>
       </c>
@@ -11552,7 +11553,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>330</v>
       </c>
@@ -11575,7 +11576,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>332</v>
       </c>
@@ -11598,7 +11599,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
       <c r="C24" s="2"/>
@@ -11607,7 +11608,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="13"/>
       <c r="C25" s="2"/>
@@ -11616,7 +11617,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="13"/>
       <c r="C26" s="2"/>
@@ -11625,7 +11626,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
       <c r="C27" s="2"/>
@@ -11634,7 +11635,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="13"/>
       <c r="C28" s="2"/>

</xml_diff>

<commit_message>
finding SS=0 for turbidity threshold
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Spring2023.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Spring2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD797D4F-2328-4168-B51C-71503CDA0D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC84C11-3F38-432A-A36E-A2C0523A5398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{99C89BF0-5701-4EDE-976A-2DC8AC06B2E1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="455">
   <si>
     <t>-</t>
   </si>
@@ -1391,6 +1391,21 @@
   </si>
   <si>
     <t>GSSIDE</t>
+  </si>
+  <si>
+    <t>Turb</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>median</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1755,6 +1770,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5454,16 +5471,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10087,10 +10104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47770336-139B-4E1D-B90D-A41F00945441}">
-  <dimension ref="A2:P156"/>
+  <dimension ref="A2:W156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R79" sqref="R79"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10112,8 +10129,12 @@
     <col min="15" max="15" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>6</v>
       </c>
@@ -10158,7 +10179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -10205,7 +10226,7 @@
         <v>81.800000000000011</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -10252,7 +10273,7 @@
         <v>51.72</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
@@ -10299,7 +10320,7 @@
         <v>91.46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -10349,7 +10370,7 @@
         <v>58.709999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>14</v>
       </c>
@@ -10396,8 +10417,11 @@
       <c r="P8" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>16</v>
       </c>
@@ -10444,8 +10468,11 @@
       <c r="P9" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>5.7697015333333299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
@@ -10493,7 +10520,7 @@
         <v>56.024999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
@@ -10541,7 +10568,7 @@
         <v>66.137500000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -10589,7 +10616,7 @@
         <v>57.156666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>26</v>
       </c>
@@ -10637,7 +10664,7 @@
         <v>47.137500000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>27</v>
       </c>
@@ -10684,8 +10711,11 @@
       <c r="P14" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>10.820681333333299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>28</v>
       </c>
@@ -10732,8 +10762,11 @@
       <c r="P15" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>16.381029333333299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>29</v>
       </c>
@@ -10781,7 +10814,7 @@
         <v>38.814999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>30</v>
       </c>
@@ -10829,7 +10862,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>40</v>
       </c>
@@ -10876,8 +10909,11 @@
       <c r="P18" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="58">
+        <v>11.302605</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>41</v>
       </c>
@@ -10924,8 +10960,11 @@
       <c r="P19" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="58">
+        <v>12.379865893333299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>42</v>
       </c>
@@ -10972,8 +11011,18 @@
       <c r="P20" s="34">
         <v>58.21</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S20" t="s">
+        <v>451</v>
+      </c>
+      <c r="T20">
+        <f>MIN(W20:W68)</f>
+        <v>4.5956702079999996</v>
+      </c>
+      <c r="W20">
+        <v>5.7697015333333299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>43</v>
       </c>
@@ -11020,8 +11069,21 @@
       <c r="P21" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>7.9286783333333304</v>
+      </c>
+      <c r="S21" t="s">
+        <v>452</v>
+      </c>
+      <c r="T21">
+        <f>MAX(W20:W68)</f>
+        <v>20.852958666666598</v>
+      </c>
+      <c r="W21">
+        <v>10.820681333333299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>44</v>
       </c>
@@ -11068,8 +11130,21 @@
       <c r="P22" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>9.2900002666666595</v>
+      </c>
+      <c r="S22" t="s">
+        <v>453</v>
+      </c>
+      <c r="T22">
+        <f>AVERAGE(W20:W68)</f>
+        <v>9.3374502056394419</v>
+      </c>
+      <c r="W22">
+        <v>16.381029333333299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>45</v>
       </c>
@@ -11116,8 +11191,18 @@
       <c r="P23" s="34">
         <v>75.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S23" t="s">
+        <v>454</v>
+      </c>
+      <c r="T23">
+        <f>MEDIAN(W20:W68)</f>
+        <v>8.70769666666666</v>
+      </c>
+      <c r="W23" s="58">
+        <v>11.302605</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>47</v>
       </c>
@@ -11164,8 +11249,14 @@
       <c r="P24" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>10.3409056666666</v>
+      </c>
+      <c r="W24" s="58">
+        <v>12.379865893333299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>48</v>
       </c>
@@ -11212,8 +11303,11 @@
       <c r="P25" s="34">
         <v>80.920000000000016</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W25">
+        <v>7.9286783333333304</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>51</v>
       </c>
@@ -11262,8 +11356,14 @@
       <c r="P26" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>6.6124433333333297</v>
+      </c>
+      <c r="W26">
+        <v>9.2900002666666595</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>52</v>
       </c>
@@ -11310,8 +11410,11 @@
       <c r="P27" s="34">
         <v>65.026666666666657</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W27">
+        <v>10.3409056666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>55</v>
       </c>
@@ -11358,8 +11461,11 @@
       <c r="P28" s="34">
         <v>59.204999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W28">
+        <v>6.6124433333333297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>59</v>
       </c>
@@ -11406,8 +11512,14 @@
       <c r="P29" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>6.3972824666666597</v>
+      </c>
+      <c r="W29">
+        <v>6.3972824666666597</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>61</v>
       </c>
@@ -11454,8 +11566,14 @@
       <c r="P30" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>6.9635272666666603</v>
+      </c>
+      <c r="W30">
+        <v>6.9635272666666603</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>62</v>
       </c>
@@ -11502,8 +11620,14 @@
       <c r="P31" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>11.1684686666666</v>
+      </c>
+      <c r="W31">
+        <v>11.1684686666666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>63</v>
       </c>
@@ -11550,8 +11674,14 @@
       <c r="P32" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>8.2048614000000004</v>
+      </c>
+      <c r="W32">
+        <v>8.2048614000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>67</v>
       </c>
@@ -11597,8 +11727,11 @@
       <c r="P33" s="34">
         <v>69.806666666666658</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W33">
+        <v>6.5715940000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>69</v>
       </c>
@@ -11647,8 +11780,14 @@
       <c r="P34" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>6.5715940000000002</v>
+      </c>
+      <c r="W34" s="59">
+        <v>7.3385368</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>71</v>
       </c>
@@ -11694,8 +11833,11 @@
       <c r="P35" s="34">
         <v>59.133333333333333</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W35">
+        <v>8.66325026666666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>75</v>
       </c>
@@ -11744,8 +11886,11 @@
       <c r="P36" s="34">
         <v>48.05</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W36">
+        <v>10.072311133333301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>77</v>
       </c>
@@ -11791,8 +11936,11 @@
       <c r="P37" s="34">
         <v>25.344999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W37">
+        <v>6.9584305310000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>80</v>
       </c>
@@ -11838,8 +11986,14 @@
       <c r="P38" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38" s="59">
+        <v>7.3385368</v>
+      </c>
+      <c r="W38">
+        <v>6.6294694666666603</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>81</v>
       </c>
@@ -11885,8 +12039,14 @@
       <c r="P39" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>8.66325026666666</v>
+      </c>
+      <c r="W39">
+        <v>5.5344294666666602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>83</v>
       </c>
@@ -11932,8 +12092,14 @@
       <c r="P40" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>10.072311133333301</v>
+      </c>
+      <c r="W40">
+        <v>5.7944035333333304</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>85</v>
       </c>
@@ -11979,8 +12145,14 @@
       <c r="P41" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>6.9584305310000003</v>
+      </c>
+      <c r="W41">
+        <v>6.8484111333333297</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>87</v>
       </c>
@@ -12026,8 +12198,14 @@
       <c r="P42" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>6.6294694666666603</v>
+      </c>
+      <c r="W42">
+        <v>8.7752321066666603</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>88</v>
       </c>
@@ -12073,8 +12251,14 @@
       <c r="P43" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>5.5344294666666602</v>
+      </c>
+      <c r="W43">
+        <v>8.5553027999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>89</v>
       </c>
@@ -12120,8 +12304,14 @@
       <c r="P44" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>5.7944035333333304</v>
+      </c>
+      <c r="W44">
+        <v>8.3964748666666598</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
@@ -12167,8 +12357,14 @@
       <c r="P45" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>6.8484111333333297</v>
+      </c>
+      <c r="W45">
+        <v>11.483500266666599</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>77</v>
       </c>
@@ -12214,8 +12410,14 @@
       <c r="P46" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>8.7752321066666603</v>
+      </c>
+      <c r="W46">
+        <v>5.4046995333333303</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
@@ -12261,8 +12463,14 @@
       <c r="P47" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>8.5553027999999998</v>
+      </c>
+      <c r="W47" s="59">
+        <v>5.62346873333333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>99</v>
       </c>
@@ -12308,8 +12516,14 @@
       <c r="P48" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>8.3964748666666598</v>
+      </c>
+      <c r="W48">
+        <v>6.59702113333333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>101</v>
       </c>
@@ -12355,8 +12569,14 @@
       <c r="P49" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>11.483500266666599</v>
+      </c>
+      <c r="W49">
+        <v>4.8982727333333296</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>102</v>
       </c>
@@ -12402,8 +12622,14 @@
       <c r="P50" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>5.4046995333333303</v>
+      </c>
+      <c r="W50">
+        <v>12.434267999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
         <v>104</v>
       </c>
@@ -12449,8 +12675,11 @@
       <c r="P51" s="34">
         <v>47.98</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W51">
+        <v>8.70769666666666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>106</v>
       </c>
@@ -12496,8 +12725,14 @@
       <c r="P52" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q52" s="59">
+        <v>5.62346873333333</v>
+      </c>
+      <c r="W52">
+        <v>10.258584000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -12543,8 +12778,14 @@
       <c r="P53" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <v>6.59702113333333</v>
+      </c>
+      <c r="W53">
+        <v>7.5019323999999896</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>115</v>
       </c>
@@ -12590,8 +12831,14 @@
       <c r="P54" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <v>4.8982727333333296</v>
+      </c>
+      <c r="W54">
+        <v>20.852958666666598</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>123</v>
       </c>
@@ -12637,8 +12884,14 @@
       <c r="P55" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q55">
+        <v>12.434267999999999</v>
+      </c>
+      <c r="W55">
+        <v>12.526063343999899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>106</v>
       </c>
@@ -12684,8 +12937,14 @@
       <c r="P56" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q56">
+        <v>8.70769666666666</v>
+      </c>
+      <c r="W56">
+        <v>9.3400750666666603</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>62</v>
       </c>
@@ -12731,8 +12990,14 @@
       <c r="P57" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q57">
+        <v>10.258584000000001</v>
+      </c>
+      <c r="W57">
+        <v>12.602335333333301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>81</v>
       </c>
@@ -12778,8 +13043,14 @@
       <c r="P58" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q58">
+        <v>7.5019323999999896</v>
+      </c>
+      <c r="W58">
+        <v>20.458221333333299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>115</v>
       </c>
@@ -12825,8 +13096,11 @@
       <c r="P59" s="34">
         <v>79.88</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W59">
+        <v>12.6200733333333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>133</v>
       </c>
@@ -12872,8 +13146,11 @@
       <c r="P60" s="34">
         <v>53.17</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W60">
+        <v>8.4514112000000008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>140</v>
       </c>
@@ -12919,8 +13196,14 @@
       <c r="P61" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q61">
+        <v>20.852958666666598</v>
+      </c>
+      <c r="W61">
+        <v>10.38581286</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>102</v>
       </c>
@@ -12966,8 +13249,14 @@
       <c r="P62" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q62">
+        <v>12.526063343999899</v>
+      </c>
+      <c r="W62">
+        <v>8.9650455999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>51</v>
       </c>
@@ -13013,8 +13302,14 @@
       <c r="P63" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <v>9.3400750666666603</v>
+      </c>
+      <c r="W63">
+        <v>12.044964</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>95</v>
       </c>
@@ -13060,8 +13355,14 @@
       <c r="P64" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q64">
+        <v>12.602335333333301</v>
+      </c>
+      <c r="W64">
+        <v>11.1430651333333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>142</v>
       </c>
@@ -13107,8 +13408,11 @@
       <c r="P65" s="34">
         <v>87.02</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="W65">
+        <v>7.3809661999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>9</v>
       </c>
@@ -13154,8 +13458,14 @@
       <c r="P66" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <v>20.458221333333299</v>
+      </c>
+      <c r="W66">
+        <v>10.366192399999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
         <v>102</v>
       </c>
@@ -13201,8 +13511,14 @@
       <c r="P67" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q67">
+        <v>12.6200733333333</v>
+      </c>
+      <c r="W67">
+        <v>4.5956702079999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
         <v>9</v>
       </c>
@@ -13248,8 +13564,14 @@
       <c r="P68" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q68">
+        <v>8.4514112000000008</v>
+      </c>
+      <c r="W68">
+        <v>9.1948653333333308</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
         <v>87</v>
       </c>
@@ -13295,8 +13617,11 @@
       <c r="P69" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q69">
+        <v>10.38581286</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
         <v>88</v>
       </c>
@@ -13342,8 +13667,11 @@
       <c r="P70" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q70">
+        <v>8.9650455999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>142</v>
       </c>
@@ -13390,7 +13718,7 @@
         <v>54.92</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
         <v>104</v>
       </c>
@@ -13437,7 +13765,7 @@
         <v>49.949999999999996</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>89</v>
       </c>
@@ -13483,8 +13811,11 @@
       <c r="P73" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q73">
+        <v>12.044964</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>81</v>
       </c>
@@ -13531,7 +13862,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
         <v>87</v>
       </c>
@@ -13577,8 +13908,11 @@
       <c r="P75" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q75">
+        <v>11.1430651333333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="47" t="s">
         <v>152</v>
       </c>
@@ -13624,8 +13958,11 @@
       <c r="P76" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q76">
+        <v>7.3809661999999996</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="47" t="s">
         <v>115</v>
       </c>
@@ -13672,7 +14009,7 @@
         <v>133.34</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>102</v>
       </c>
@@ -13718,8 +14055,11 @@
       <c r="P78" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q78">
+        <v>10.366192399999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -13766,7 +14106,7 @@
         <v>79.66</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>113</v>
       </c>
@@ -13813,7 +14153,7 @@
         <v>30.57</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>95</v>
       </c>
@@ -13860,7 +14200,7 @@
         <v>26.823333333333334</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>95</v>
       </c>
@@ -13907,7 +14247,7 @@
         <v>113.11</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>104</v>
       </c>
@@ -13953,8 +14293,11 @@
       <c r="P83" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q83">
+        <v>4.5956702079999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>133</v>
       </c>
@@ -14001,7 +14344,7 @@
         <v>93.39</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>101</v>
       </c>
@@ -14048,7 +14391,7 @@
         <v>44.193333333333328</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>77</v>
       </c>
@@ -14094,8 +14437,11 @@
       <c r="P86" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q86">
+        <v>9.1948653333333308</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>10</v>
       </c>
@@ -14142,7 +14488,7 @@
         <v>50.42</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>8</v>
       </c>
@@ -14166,7 +14512,7 @@
       </c>
       <c r="I88" s="29"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>155</v>
       </c>
@@ -14190,7 +14536,7 @@
       </c>
       <c r="I89" s="29"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -14214,7 +14560,7 @@
       </c>
       <c r="I90" s="29"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>156</v>
       </c>
@@ -14238,7 +14584,7 @@
       </c>
       <c r="I91" s="29"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>123</v>
       </c>
@@ -14262,7 +14608,7 @@
       </c>
       <c r="I92" s="29"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>142</v>
       </c>
@@ -14286,7 +14632,7 @@
       </c>
       <c r="I93" s="29"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="50" t="s">
         <v>69</v>
       </c>
@@ -14310,7 +14656,7 @@
       </c>
       <c r="I94" s="29"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="50" t="s">
         <v>71</v>
       </c>
@@ -14334,7 +14680,7 @@
       </c>
       <c r="I95" s="29"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="50" t="s">
         <v>75</v>
       </c>

</xml_diff>